<commit_message>
Add basic testing scripts
</commit_message>
<xml_diff>
--- a/Datasets.xlsx
+++ b/Datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tfaithfu\Github Repos\lmm_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8ECD1-6A55-409E-A139-F49FC8B12A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EFC405-4C31-4C80-8D78-FA0E6FCD26F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{45FBCF12-202C-4FD7-8B72-3E64ACF103AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
   <si>
     <t>Sub-task</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>Human ratings</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/adityajn105/flickr8k</t>
+  </si>
+  <si>
+    <t>Flickr8k</t>
+  </si>
+  <si>
+    <t>Popular caption benchmark</t>
   </si>
 </sst>
 </file>
@@ -550,65 +559,65 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -947,20 +956,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4890A2D0-AED8-465A-BAEE-48012F900F37}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44" style="10" customWidth="1"/>
-    <col min="6" max="6" width="47.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.90625" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="1" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44" style="6" customWidth="1"/>
+    <col min="6" max="6" width="47.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.90625" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -976,532 +985,542 @@
       <c r="D1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="8">
         <v>224714</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="3" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="8">
         <v>328000</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>714</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <v>3000</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="8">
         <v>47542</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="3" t="s">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
-      <c r="B25" s="2" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" s="8">
         <v>30000</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="A29" s="17"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A24:A29"/>
     <mergeCell ref="A11:G11"/>
@@ -1510,15 +1529,14 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{DDA7AF57-AE7E-4961-8426-64061FA40E2F}"/>
+    <hyperlink ref="D14" r:id="rId2" xr:uid="{29F99CE7-70DF-4C97-9199-7CE2A91B4C82}"/>
+    <hyperlink ref="D13" r:id="rId3" xr:uid="{8D145BC2-CD21-4F79-B9C8-EAB12BC72735}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{CF172E53-D51B-43F0-A8E3-4766B4BACC52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add script for captions
</commit_message>
<xml_diff>
--- a/Datasets.xlsx
+++ b/Datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tfaithfu\Github Repos\lmm_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EFC405-4C31-4C80-8D78-FA0E6FCD26F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77990E9-080A-4B2E-A73B-D6B9DEC4B846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{45FBCF12-202C-4FD7-8B72-3E64ACF103AF}"/>
   </bookViews>
@@ -598,6 +598,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,9 +617,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4890A2D0-AED8-465A-BAEE-48012F900F37}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,10 +996,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1019,8 +1019,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="21"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1059,7 +1059,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1101,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="21"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1122,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1143,7 +1143,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="21"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="21"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1175,19 +1175,19 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1207,8 +1207,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="21"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1226,8 +1226,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="21"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1245,7 +1245,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="21"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1266,16 +1266,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1284,7 +1284,7 @@
       <c r="C17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1298,8 +1298,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1319,8 +1319,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
@@ -1338,14 +1338,14 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="12" t="s">
         <v>89</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="16"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="17"/>
+      <c r="B21" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1380,12 +1380,12 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="12" t="s">
         <v>92</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -1399,16 +1399,16 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1431,8 +1431,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="17"/>
+      <c r="B25" s="16" t="s">
         <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1452,8 +1452,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1471,7 +1471,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="2" t="s">
         <v>118</v>
       </c>
@@ -1492,7 +1492,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>120</v>
@@ -1507,7 +1507,7 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="17"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1517,11 +1517,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A17:A22"/>
     <mergeCell ref="A24:A29"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A16:G16"/>
@@ -1529,14 +1524,22 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A17:A22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{DDA7AF57-AE7E-4961-8426-64061FA40E2F}"/>
     <hyperlink ref="D14" r:id="rId2" xr:uid="{29F99CE7-70DF-4C97-9199-7CE2A91B4C82}"/>
     <hyperlink ref="D13" r:id="rId3" xr:uid="{8D145BC2-CD21-4F79-B9C8-EAB12BC72735}"/>
     <hyperlink ref="D12" r:id="rId4" xr:uid="{CF172E53-D51B-43F0-A8E3-4766B4BACC52}"/>
+    <hyperlink ref="D17" r:id="rId5" xr:uid="{5CB43DB8-608B-47ED-BA8A-282099AC8ADD}"/>
+    <hyperlink ref="D22" r:id="rId6" xr:uid="{771A17FB-3A0D-45AA-A588-E883C410137D}"/>
+    <hyperlink ref="D20" r:id="rId7" xr:uid="{3F5030E3-CB0C-43D0-AD8F-0AB11EEE2C18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new benchmark scripts
</commit_message>
<xml_diff>
--- a/Datasets.xlsx
+++ b/Datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tfaithfu\Github Repos\lmm_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77990E9-080A-4B2E-A73B-D6B9DEC4B846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8645C36-6E1D-410A-A755-67747636C88A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{45FBCF12-202C-4FD7-8B72-3E64ACF103AF}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>MS COCO Captions</t>
   </si>
   <si>
-    <t>https://paperswithcode.com/dataset/coco-captions</t>
-  </si>
-  <si>
     <t>330,000 images, 5 captions per image</t>
   </si>
   <si>
@@ -403,6 +400,10 @@
   </si>
   <si>
     <t>Popular caption benchmark</t>
+  </si>
+  <si>
+    <t>https://paperswithcode.com/dataset/coco-captions
+https://huggingface.co/datasets/ChristophSchuhmann/MS_COCO_2017_URL_TEXT</t>
   </si>
 </sst>
 </file>
@@ -598,9 +599,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -617,6 +615,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -956,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4890A2D0-AED8-465A-BAEE-48012F900F37}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,10 +997,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1019,8 +1020,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
@@ -1038,7 +1039,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1059,7 +1060,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1080,7 +1081,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1101,7 +1102,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1123,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="15"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1143,7 +1144,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="15"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1154,7 +1155,7 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1175,19 +1176,19 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1207,8 +1208,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1226,8 +1227,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1245,7 +1246,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="15"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1266,16 +1267,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="19"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1298,8 +1299,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="17"/>
-      <c r="B18" s="16" t="s">
+      <c r="A18" s="16"/>
+      <c r="B18" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1319,8 +1320,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="2" t="s">
         <v>109</v>
       </c>
@@ -1338,7 +1339,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
@@ -1359,8 +1360,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="17"/>
-      <c r="B21" s="16" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1380,8 +1381,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="2" t="s">
         <v>41</v>
       </c>
@@ -1399,20 +1400,20 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>46</v>
@@ -1430,30 +1431,30 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="17"/>
-      <c r="B25" s="16" t="s">
-        <v>117</v>
+    <row r="25" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="16"/>
+      <c r="B25" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>114</v>
+      <c r="D25" s="5" t="s">
+        <v>121</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="17"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1471,9 +1472,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>50</v>
@@ -1492,22 +1493,22 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="17"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="18"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1517,6 +1518,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A17:A22"/>
     <mergeCell ref="A24:A29"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A16:G16"/>
@@ -1524,11 +1530,6 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A17:A22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D6" r:id="rId1" xr:uid="{DDA7AF57-AE7E-4961-8426-64061FA40E2F}"/>

</xml_diff>